<commit_message>
Implemented with apache poi library and change drvier to read from excel
</commit_message>
<xml_diff>
--- a/src/main/scala/dataEngine/DataEngine.xlsx
+++ b/src/main/scala/dataEngine/DataEngine.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Action_Keyword</t>
+    <t xml:space="preserve">ActionKeyword</t>
   </si>
   <si>
     <t xml:space="preserve">Login_01</t>
@@ -40,37 +40,37 @@
     <t xml:space="preserve">TS_0001</t>
   </si>
   <si>
-    <t xml:space="preserve">Open the Browser </t>
-  </si>
-  <si>
-    <t xml:space="preserve">openBrowser</t>
+    <t xml:space="preserve">Navigate to website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigate</t>
   </si>
   <si>
     <t xml:space="preserve">TS_0002</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigate to website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navigate</t>
+    <t xml:space="preserve">Enter the Username in the Username field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inputUsername</t>
   </si>
   <si>
     <t xml:space="preserve">TS_0003</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter the Username in the Username field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">input_Username</t>
+    <t xml:space="preserve">Enter the Password in the Password field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inputPassword</t>
   </si>
   <si>
     <t xml:space="preserve">TS_0004</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter the Password in the Password field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">input_Password</t>
+    <t xml:space="preserve">Close the browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closeBrowser</t>
   </si>
 </sst>
 </file>
@@ -170,7 +170,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>